<commit_message>
Added purple urchin samples to RawSizeMass prey table, plus some very minor tweaks to Boutprocess and Fdatprocess
</commit_message>
<xml_diff>
--- a/preylib/Species.xlsx
+++ b/preylib/Species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/SOFA2/SOFA/preylib/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhydra-my.sharepoint.com/personal/ttinker_nhydra-eco_com/Documents/SOFA2/SOFA/preylib/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{A23D99A9-694F-4699-A28C-CA127BD4CD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BC1DFD3-B2E6-4328-9876-C1932C2385B7}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="740" windowWidth="23980" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6390" yWindow="1785" windowWidth="37320" windowHeight="18315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="1" r:id="rId1"/>
@@ -8321,32 +8321,32 @@
   <dimension ref="A1:R144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G99" sqref="G99"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" customWidth="1"/>
-    <col min="7" max="7" width="25.81640625" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="30.54296875" style="4" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="13.7265625" customWidth="1"/>
-    <col min="12" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="8.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.54296875" customWidth="1"/>
-    <col min="18" max="18" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8402,7 +8402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8446,7 +8446,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>79118</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8548,7 +8548,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8636,7 +8636,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8665,7 +8665,7 @@
         <v>79452</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -8694,7 +8694,7 @@
         <v>81446</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -8738,7 +8738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -8826,7 +8826,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
@@ -8870,7 +8870,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
@@ -8917,7 +8917,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>16</v>
       </c>
@@ -8949,7 +8949,7 @@
         <v>98670</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>17</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>18</v>
       </c>
@@ -9001,7 +9001,7 @@
         <v>79451</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>19</v>
       </c>
@@ -9042,7 +9042,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -9086,7 +9086,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>22</v>
       </c>
@@ -9171,7 +9171,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>24</v>
       </c>
@@ -9215,7 +9215,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>25</v>
       </c>
@@ -9259,7 +9259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>26</v>
       </c>
@@ -9300,7 +9300,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>27</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>98435</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>28</v>
       </c>
@@ -9370,7 +9370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>29</v>
       </c>
@@ -9411,7 +9411,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>30</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>31</v>
       </c>
@@ -9496,7 +9496,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>32</v>
       </c>
@@ -9522,7 +9522,7 @@
         <v>157968</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>33</v>
       </c>
@@ -9563,7 +9563,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>34</v>
       </c>
@@ -9604,7 +9604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>35</v>
       </c>
@@ -9645,7 +9645,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>36</v>
       </c>
@@ -9686,7 +9686,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>37</v>
       </c>
@@ -9709,7 +9709,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>38</v>
       </c>
@@ -9753,7 +9753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>39</v>
       </c>
@@ -9797,7 +9797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>40</v>
       </c>
@@ -9826,7 +9826,7 @@
         <v>81033</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>41</v>
       </c>
@@ -9873,7 +9873,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>42</v>
       </c>
@@ -9920,7 +9920,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>43</v>
       </c>
@@ -9964,7 +9964,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>44</v>
       </c>
@@ -10005,7 +10005,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>45</v>
       </c>
@@ -10037,7 +10037,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>46</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>47</v>
       </c>
@@ -10122,7 +10122,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>48</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>49</v>
       </c>
@@ -10201,7 +10201,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>50</v>
       </c>
@@ -10242,7 +10242,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>51</v>
       </c>
@@ -10286,7 +10286,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>52</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>53</v>
       </c>
@@ -10368,7 +10368,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>54</v>
       </c>
@@ -10394,7 +10394,7 @@
         <v>64358</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>55</v>
       </c>
@@ -10438,7 +10438,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>56</v>
       </c>
@@ -10467,7 +10467,7 @@
         <v>79612</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>57</v>
       </c>
@@ -10493,7 +10493,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>58</v>
       </c>
@@ -10537,7 +10537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>59</v>
       </c>
@@ -10581,7 +10581,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>60</v>
       </c>
@@ -10622,7 +10622,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>61</v>
       </c>
@@ -10663,7 +10663,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>62</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>63</v>
       </c>
@@ -10749,7 +10749,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>64</v>
       </c>
@@ -10778,7 +10778,7 @@
         <v>81691</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>65</v>
       </c>
@@ -10823,7 +10823,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>66</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>67</v>
       </c>
@@ -10899,7 +10899,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>68</v>
       </c>
@@ -10949,7 +10949,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>69</v>
       </c>
@@ -10990,7 +10990,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>70</v>
       </c>
@@ -11016,7 +11016,7 @@
         <v>156862</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>71</v>
       </c>
@@ -11051,7 +11051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>72</v>
       </c>
@@ -11086,7 +11086,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>73</v>
       </c>
@@ -11130,7 +11130,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>74</v>
       </c>
@@ -11165,7 +11165,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>75</v>
       </c>
@@ -11200,7 +11200,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>76</v>
       </c>
@@ -11238,7 +11238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>77</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>158140</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>78</v>
       </c>
@@ -11290,7 +11290,7 @@
         <v>158191</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>79</v>
       </c>
@@ -11334,7 +11334,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>80</v>
       </c>
@@ -11360,7 +11360,7 @@
         <v>166082</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>81</v>
       </c>
@@ -11404,7 +11404,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>82</v>
       </c>
@@ -11442,7 +11442,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>83</v>
       </c>
@@ -11465,7 +11465,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>84</v>
       </c>
@@ -11509,7 +11509,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>85</v>
       </c>
@@ -11550,7 +11550,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>86</v>
       </c>
@@ -11573,7 +11573,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>87</v>
       </c>
@@ -11614,7 +11614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>88</v>
       </c>
@@ -11658,7 +11658,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>89</v>
       </c>
@@ -11687,7 +11687,7 @@
         <v>97775</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>90</v>
       </c>
@@ -11728,7 +11728,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>92</v>
       </c>
@@ -11766,7 +11766,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="90" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>93</v>
       </c>
@@ -11810,7 +11810,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>94</v>
       </c>
@@ -11851,7 +11851,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>95</v>
       </c>
@@ -11889,7 +11889,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>96</v>
       </c>
@@ -11927,7 +11927,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>97</v>
       </c>
@@ -11968,7 +11968,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>98</v>
       </c>
@@ -12009,7 +12009,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="96" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>99</v>
       </c>
@@ -12053,7 +12053,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>100</v>
       </c>
@@ -12094,7 +12094,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>101</v>
       </c>
@@ -12132,7 +12132,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="99" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>102</v>
       </c>
@@ -12173,7 +12173,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="100" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>103</v>
       </c>
@@ -12211,7 +12211,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>104</v>
       </c>
@@ -12252,7 +12252,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>105</v>
       </c>
@@ -12293,7 +12293,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>106</v>
       </c>
@@ -12334,7 +12334,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="104" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>107</v>
       </c>
@@ -12381,7 +12381,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="105" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>108</v>
       </c>
@@ -12422,7 +12422,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>109</v>
       </c>
@@ -12463,7 +12463,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>110</v>
       </c>
@@ -12510,7 +12510,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="108" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>111</v>
       </c>
@@ -12554,7 +12554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>112</v>
       </c>
@@ -12595,7 +12595,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="110" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>113</v>
       </c>
@@ -12636,7 +12636,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>114</v>
       </c>
@@ -12680,7 +12680,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>115</v>
       </c>
@@ -12724,7 +12724,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>116</v>
       </c>
@@ -12765,7 +12765,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>117</v>
       </c>
@@ -12806,7 +12806,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>118</v>
       </c>
@@ -12853,7 +12853,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>119</v>
       </c>
@@ -12894,7 +12894,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>120</v>
       </c>
@@ -12938,7 +12938,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>121</v>
       </c>
@@ -12982,7 +12982,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>122</v>
       </c>
@@ -13026,7 +13026,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>123</v>
       </c>
@@ -13070,7 +13070,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>124</v>
       </c>
@@ -13111,7 +13111,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>125</v>
       </c>
@@ -13152,7 +13152,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>126</v>
       </c>
@@ -13187,7 +13187,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>127</v>
       </c>
@@ -13225,7 +13225,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>128</v>
       </c>
@@ -13266,7 +13266,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="126" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>129</v>
       </c>
@@ -13302,7 +13302,7 @@
       </c>
       <c r="R126" s="6"/>
     </row>
-    <row r="127" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>130</v>
       </c>
@@ -13341,7 +13341,7 @@
       </c>
       <c r="R127" s="6"/>
     </row>
-    <row r="128" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>131</v>
       </c>
@@ -13379,7 +13379,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>132</v>
       </c>
@@ -13418,7 +13418,7 @@
       </c>
       <c r="R129" s="6"/>
     </row>
-    <row r="130" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>133</v>
       </c>
@@ -13462,7 +13462,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>134</v>
       </c>
@@ -13506,7 +13506,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>135</v>
       </c>
@@ -13550,7 +13550,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="133" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>136</v>
       </c>
@@ -13594,7 +13594,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>137</v>
       </c>
@@ -13635,7 +13635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>138</v>
       </c>
@@ -13673,7 +13673,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>139</v>
       </c>
@@ -13714,7 +13714,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="137" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>140</v>
       </c>
@@ -13755,7 +13755,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>141</v>
       </c>
@@ -13796,7 +13796,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>142</v>
       </c>
@@ -13837,7 +13837,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>143</v>
       </c>
@@ -13878,7 +13878,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>144</v>
       </c>
@@ -13922,7 +13922,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>145</v>
       </c>
@@ -13963,7 +13963,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>146</v>
       </c>
@@ -14001,7 +14001,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>147</v>
       </c>
@@ -14049,6 +14049,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007C85BEB69FC2D74FAF0CFFD217B4FC14" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="710db677ec6c1f9e2ee7ec057b94e111">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6188df5f-cd89-4f8d-a557-25c3c9ac281d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b477d7946c345dc1bd1ea843bd6a9161" ns2:_="">
     <xsd:import namespace="6188df5f-cd89-4f8d-a557-25c3c9ac281d"/>
@@ -14180,12 +14186,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{701BD999-73B0-4962-BCE6-126EFE86DF99}">
   <ds:schemaRefs>
@@ -14195,6 +14195,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD505C4D-7CBD-4BA9-BA76-7F323588199A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6188df5f-cd89-4f8d-a557-25c3c9ac281d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC9E02A9-0E2F-49B5-9C17-D38DD2951BA2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14210,20 +14226,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD505C4D-7CBD-4BA9-BA76-7F323588199A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6188df5f-cd89-4f8d-a557-25c3c9ac281d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>